<commit_message>
bug fix with import
</commit_message>
<xml_diff>
--- a/uids.xlsx
+++ b/uids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreykarganov/Desktop/Work/skud_2.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478EE0C2-F143-F847-BE2C-FA3BE6A50310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614D19DC-F933-2E44-901E-AF2B39F40733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11880" yWindow="2400" windowWidth="27840" windowHeight="16740" xr2:uid="{0B284FE5-E93D-E841-A06E-31407582DE0F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="98">
   <si>
     <t>Амер Александр Таирович</t>
   </si>
@@ -323,6 +323,12 @@
   </si>
   <si>
     <t>С/с-22-3-о</t>
+  </si>
+  <si>
+    <t>nothing1</t>
+  </si>
+  <si>
+    <t>Чеченцев Герман Эльклассико</t>
   </si>
 </sst>
 </file>
@@ -675,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C1DA97F-2DC0-B341-BFC1-D68E2342A65B}">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1530,6 +1536,17 @@
         <v>83</v>
       </c>
     </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>96</v>
+      </c>
+      <c r="B78" t="s">
+        <v>97</v>
+      </c>
+      <c r="C78" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>